<commit_message>
ERD modified. Test cases for Employees and Customers completed. Doc for the final project started.
</commit_message>
<xml_diff>
--- a/Relational Data Model/Relational Data Model.xlsx
+++ b/Relational Data Model/Relational Data Model.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JohnA\Documents\Lambton College\Spring Term 2023\CSD-2206 Database Design and SQL\Assignments\Fianl Project\Relational Data Model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JohnA\Documents\Lambton College\Spring Term 2023\CSD-2206 Database Design and SQL\Assignments\Final Project\Relational Data Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F02E3E5-8EE4-4DB3-A792-33FB45D605BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF930250-513D-441C-B25D-A15347017C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{95CE2CC2-7658-41BA-ACF3-9B6548654C82}"/>
   </bookViews>
@@ -167,9 +167,6 @@
     <t>craft_name</t>
   </si>
   <si>
-    <t>(7,2)</t>
-  </si>
-  <si>
     <t>selling_price</t>
   </si>
   <si>
@@ -239,9 +236,6 @@
     <t>ZIPS</t>
   </si>
   <si>
-    <t>WAREHOUSE</t>
-  </si>
-  <si>
     <t>Datatype</t>
   </si>
   <si>
@@ -257,9 +251,6 @@
     <t>(8,2)</t>
   </si>
   <si>
-    <t>ORDER</t>
-  </si>
-  <si>
     <t>Key type</t>
   </si>
   <si>
@@ -357,6 +348,15 @@
   </si>
   <si>
     <t>emp_status</t>
+  </si>
+  <si>
+    <t>(9,2)</t>
+  </si>
+  <si>
+    <t>WAREHOUSES</t>
+  </si>
+  <si>
+    <t>ORDERS</t>
   </si>
 </sst>
 </file>
@@ -822,8 +822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F0A6DEB-4CD2-4B0A-BB02-28B5EA6F7998}">
   <dimension ref="A1:E142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C140" sqref="C140"/>
+    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I127" sqref="I127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -834,7 +834,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -901,7 +901,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
@@ -983,7 +983,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
@@ -1050,7 +1050,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
@@ -1120,7 +1120,7 @@
         <v>9</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -1132,7 +1132,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -1209,7 +1209,7 @@
         <v>7</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>24</v>
@@ -1227,7 +1227,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
@@ -1265,7 +1265,7 @@
         <v>9</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -1339,7 +1339,7 @@
         <v>7</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>24</v>
@@ -1354,7 +1354,7 @@
         <v>7</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>24</v>
@@ -1369,7 +1369,7 @@
         <v>7</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>24</v>
@@ -1384,13 +1384,13 @@
         <v>7</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -1399,7 +1399,7 @@
         <v>7</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>24</v>
@@ -1414,7 +1414,7 @@
         <v>15</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>24</v>
@@ -1470,7 +1470,7 @@
         <v>9</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
@@ -1502,7 +1502,7 @@
         <v>9</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -1527,7 +1527,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B52" s="12"/>
       <c r="C52" s="12"/>
@@ -1713,7 +1713,7 @@
         <v>15</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>9</v>
@@ -1758,7 +1758,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B68" s="12"/>
       <c r="C68" s="12"/>
@@ -1820,13 +1820,13 @@
         <v>7</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D72" s="6" t="s">
         <v>9</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>43</v>
+        <v>104</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
@@ -1835,13 +1835,13 @@
         <v>7</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D73" s="6" t="s">
         <v>9</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>43</v>
+        <v>104</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
@@ -1850,7 +1850,7 @@
         <v>7</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>24</v>
@@ -1865,7 +1865,7 @@
         <v>15</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>24</v>
@@ -1880,7 +1880,7 @@
         <v>7</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>24</v>
@@ -1895,7 +1895,7 @@
         <v>7</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>24</v>
@@ -1910,7 +1910,7 @@
         <v>15</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>24</v>
@@ -1921,7 +1921,7 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B81" s="9"/>
       <c r="C81" s="9"/>
@@ -1959,7 +1959,7 @@
         <v>9</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>24</v>
@@ -1985,7 +1985,7 @@
         <v>7</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>24</v>
@@ -2017,7 +2017,7 @@
         <v>15</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>24</v>
@@ -2066,7 +2066,7 @@
         <v>15</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D90" s="6" t="s">
         <v>9</v>
@@ -2077,7 +2077,7 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B92" s="9"/>
       <c r="C92" s="9"/>
@@ -2124,7 +2124,7 @@
         <v>7</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>24</v>
@@ -2139,7 +2139,7 @@
         <v>7</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>24</v>
@@ -2154,7 +2154,7 @@
         <v>7</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>24</v>
@@ -2165,7 +2165,7 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" s="11" t="s">
-        <v>67</v>
+        <v>105</v>
       </c>
       <c r="B99" s="12"/>
       <c r="C99" s="12"/>
@@ -2183,7 +2183,7 @@
         <v>3</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E100" s="5" t="s">
         <v>5</v>
@@ -2212,7 +2212,7 @@
         <v>7</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>24</v>
@@ -2242,13 +2242,13 @@
         <v>7</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D104" s="6" t="s">
         <v>9</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
@@ -2270,7 +2270,7 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" s="11" t="s">
-        <v>73</v>
+        <v>106</v>
       </c>
       <c r="B107" s="12"/>
       <c r="C107" s="12"/>
@@ -2279,19 +2279,19 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B108" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D108" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E108" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
@@ -2308,7 +2308,7 @@
         <v>9</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
@@ -2317,7 +2317,7 @@
         <v>7</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>12</v>
@@ -2330,7 +2330,7 @@
         <v>7</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>12</v>
@@ -2343,7 +2343,7 @@
         <v>7</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D112" s="1" t="s">
         <v>24</v>
@@ -2377,7 +2377,7 @@
         <v>7</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D114" s="6" t="s">
         <v>9</v>
@@ -2392,7 +2392,7 @@
         <v>7</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>24</v>
@@ -2403,7 +2403,7 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" s="11" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B117" s="12"/>
       <c r="C117" s="12"/>
@@ -2412,19 +2412,19 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B118" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D118" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E118" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.3">
@@ -2435,7 +2435,7 @@
         <v>7</v>
       </c>
       <c r="C119" s="6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D119" s="6" t="s">
         <v>9</v>
@@ -2516,7 +2516,7 @@
         <v>9</v>
       </c>
       <c r="E124" s="6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
@@ -2542,7 +2542,7 @@
         <v>15</v>
       </c>
       <c r="C126" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D126" s="6" t="s">
         <v>12</v>
@@ -2555,13 +2555,13 @@
         <v>7</v>
       </c>
       <c r="C127" s="6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D127" s="6" t="s">
         <v>9</v>
       </c>
       <c r="E127" s="6" t="s">
-        <v>43</v>
+        <v>104</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.3">
@@ -2570,7 +2570,7 @@
         <v>7</v>
       </c>
       <c r="C128" s="6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D128" s="6" t="s">
         <v>24</v>
@@ -2587,7 +2587,7 @@
         <v>15</v>
       </c>
       <c r="C129" s="6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D129" s="6" t="s">
         <v>9</v>
@@ -2621,7 +2621,7 @@
         <v>15</v>
       </c>
       <c r="C131" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D131" s="6" t="s">
         <v>9</v>
@@ -2649,7 +2649,7 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" s="8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B134" s="9"/>
       <c r="C134" s="9"/>
@@ -2658,19 +2658,19 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B135" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C135" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D135" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E135" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
@@ -2681,7 +2681,7 @@
         <v>7</v>
       </c>
       <c r="C136" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D136" s="6" t="s">
         <v>9</v>
@@ -2698,7 +2698,7 @@
         <v>7</v>
       </c>
       <c r="C137" s="6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D137" s="6" t="s">
         <v>24</v>
@@ -2715,7 +2715,7 @@
         <v>7</v>
       </c>
       <c r="C138" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D138" s="6" t="s">
         <v>24</v>
@@ -2732,7 +2732,7 @@
         <v>7</v>
       </c>
       <c r="C139" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D139" s="6" t="s">
         <v>24</v>
@@ -2747,13 +2747,13 @@
         <v>7</v>
       </c>
       <c r="C140" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D140" s="6" t="s">
         <v>9</v>
       </c>
       <c r="E140" s="6" t="s">
-        <v>43</v>
+        <v>104</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.3">
@@ -2762,7 +2762,7 @@
         <v>15</v>
       </c>
       <c r="C141" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D141" s="6" t="s">
         <v>24</v>
@@ -2779,7 +2779,7 @@
         <v>15</v>
       </c>
       <c r="C142" s="6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D142" s="6" t="s">
         <v>9</v>
@@ -2790,6 +2790,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="A23:E23"/>
     <mergeCell ref="A134:E134"/>
     <mergeCell ref="A30:E30"/>
     <mergeCell ref="A92:E92"/>
@@ -2801,11 +2806,6 @@
     <mergeCell ref="A107:E107"/>
     <mergeCell ref="A117:E117"/>
     <mergeCell ref="A35:E35"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A17:E17"/>
-    <mergeCell ref="A23:E23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>